<commit_message>
Updated ERM Keywords and erm Files
</commit_message>
<xml_diff>
--- a/app/data/pools/erm.xlsx
+++ b/app/data/pools/erm.xlsx
@@ -1,29 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21629"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\discovery\app\data\pools\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C69C7EA-16FB-409C-8532-0F8CBBBA1CFF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="7410" tabRatio="500"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" firstSheet="1" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ERM Vendors Master File" sheetId="20" r:id="rId1"/>
-    <sheet name="E1-Desktop Applications" sheetId="1" r:id="rId2"/>
-    <sheet name="E2-Electronic Messages" sheetId="10" r:id="rId3"/>
-    <sheet name="E3-Social Media" sheetId="11" r:id="rId4"/>
-    <sheet name="E4-Cloud Services" sheetId="12" r:id="rId5"/>
-    <sheet name="E5-Websites" sheetId="13" r:id="rId6"/>
-    <sheet name="E6-Digital Media (Photo)" sheetId="14" r:id="rId7"/>
-    <sheet name="E7-Digital Media (Audio)" sheetId="15" r:id="rId8"/>
-    <sheet name="E8-Digital Media (Video)" sheetId="16" r:id="rId9"/>
-    <sheet name="E9-Databases" sheetId="17" r:id="rId10"/>
-    <sheet name="E10-Shared Drives" sheetId="18" r:id="rId11"/>
-    <sheet name="E11-Engineering Drawings" sheetId="19" r:id="rId12"/>
+    <sheet name="E(1)-Desktop Applications" sheetId="1" r:id="rId2"/>
+    <sheet name="E(2)-Electronic Messages" sheetId="10" r:id="rId3"/>
+    <sheet name="E(3)-Social Media" sheetId="11" r:id="rId4"/>
+    <sheet name="E(4)-Cloud Services" sheetId="12" r:id="rId5"/>
+    <sheet name="E(5)-Websites" sheetId="13" r:id="rId6"/>
+    <sheet name="E(6)-Digital Media (Photo)" sheetId="14" r:id="rId7"/>
+    <sheet name="E(7)-Digital Media (Audio)" sheetId="15" r:id="rId8"/>
+    <sheet name="E(8)-Digital Media (Video)" sheetId="16" r:id="rId9"/>
+    <sheet name="E(9)-Databases" sheetId="17" r:id="rId10"/>
+    <sheet name="E(10)-Shared Drives" sheetId="18" r:id="rId11"/>
+    <sheet name="E(11)-Engineering Drawings" sheetId="19" r:id="rId12"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'ERM Vendors Master File'!$A$1:$AK$46</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="181029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -801,7 +814,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1148,11 +1161,11 @@
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text 2" xfId="4"/>
+    <cellStyle name="Explanatory Text 2" xfId="4" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="3"/>
-    <cellStyle name="Normal 3" xfId="2"/>
+    <cellStyle name="Normal 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="Normal 3" xfId="2" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1228,6 +1241,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -1275,7 +1291,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1308,9 +1324,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1343,6 +1376,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1518,10 +1568,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AK46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>
@@ -5607,10 +5657,10 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AK46"/>
+  <autoFilter ref="A1:AK46" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <hyperlinks>
-    <hyperlink ref="F3" r:id="rId1" display="mailto:andrewm@aitheras.com"/>
-    <hyperlink ref="I3" r:id="rId2" display="mailto:denise.muir@aitheras.com"/>
+    <hyperlink ref="F3" r:id="rId1" display="mailto:andrewm@aitheras.com" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="I3" r:id="rId2" display="mailto:denise.muir@aitheras.com" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
@@ -5618,10 +5668,10 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:Y42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A30" sqref="A30:XFD30"/>
     </sheetView>
   </sheetViews>
@@ -8005,19 +8055,19 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F3" r:id="rId1" display="mailto:andrewm@aitheras.com"/>
-    <hyperlink ref="I3" r:id="rId2" display="mailto:denise.muir@aitheras.com"/>
+    <hyperlink ref="F3" r:id="rId1" display="mailto:andrewm@aitheras.com" xr:uid="{00000000-0004-0000-0900-000000000000}"/>
+    <hyperlink ref="I3" r:id="rId2" display="mailto:denise.muir@aitheras.com" xr:uid="{00000000-0004-0000-0900-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:Y38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A28" sqref="A28:XFD28"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="J39" sqref="J39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -10166,19 +10216,19 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F3" r:id="rId1" display="mailto:andrewm@aitheras.com"/>
-    <hyperlink ref="I3" r:id="rId2" display="mailto:denise.muir@aitheras.com"/>
+    <hyperlink ref="F3" r:id="rId1" display="mailto:andrewm@aitheras.com" xr:uid="{00000000-0004-0000-0A00-000000000000}"/>
+    <hyperlink ref="I3" r:id="rId2" display="mailto:denise.muir@aitheras.com" xr:uid="{00000000-0004-0000-0A00-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:Y40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+      <selection activeCell="H33" sqref="H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -12415,18 +12465,18 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F3" r:id="rId1" display="mailto:andrewm@aitheras.com"/>
-    <hyperlink ref="I3" r:id="rId2" display="mailto:denise.muir@aitheras.com"/>
+    <hyperlink ref="F3" r:id="rId1" display="mailto:andrewm@aitheras.com" xr:uid="{00000000-0004-0000-0B00-000000000000}"/>
+    <hyperlink ref="I3" r:id="rId2" display="mailto:denise.muir@aitheras.com" xr:uid="{00000000-0004-0000-0B00-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AB41"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A29" sqref="A29:XFD29"/>
     </sheetView>
   </sheetViews>
@@ -14801,8 +14851,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F3" r:id="rId1" display="mailto:andrewm@aitheras.com"/>
-    <hyperlink ref="I3" r:id="rId2" display="mailto:denise.muir@aitheras.com"/>
+    <hyperlink ref="F3" r:id="rId1" display="mailto:andrewm@aitheras.com" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="I3" r:id="rId2" display="mailto:denise.muir@aitheras.com" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
@@ -14810,11 +14860,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AB40"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30:XFD30"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -17095,8 +17145,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F3" r:id="rId1" display="mailto:andrewm@aitheras.com"/>
-    <hyperlink ref="I3" r:id="rId2" display="mailto:denise.muir@aitheras.com"/>
+    <hyperlink ref="F3" r:id="rId1" display="mailto:andrewm@aitheras.com" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="I3" r:id="rId2" display="mailto:denise.muir@aitheras.com" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
@@ -17104,7 +17154,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AB35"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -19129,11 +19179,11 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AB41"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30:XFD30"/>
+      <selection activeCell="I32" sqref="I32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -21489,8 +21539,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F3" r:id="rId1" display="mailto:andrewm@aitheras.com"/>
-    <hyperlink ref="I3" r:id="rId2" display="mailto:denise.muir@aitheras.com"/>
+    <hyperlink ref="F3" r:id="rId1" display="mailto:andrewm@aitheras.com" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
+    <hyperlink ref="I3" r:id="rId2" display="mailto:denise.muir@aitheras.com" xr:uid="{00000000-0004-0000-0400-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
@@ -21498,7 +21548,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:AB37"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -23636,8 +23686,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F3" r:id="rId1" display="mailto:andrewm@aitheras.com"/>
-    <hyperlink ref="I3" r:id="rId2" display="mailto:denise.muir@aitheras.com"/>
+    <hyperlink ref="F3" r:id="rId1" display="mailto:andrewm@aitheras.com" xr:uid="{00000000-0004-0000-0500-000000000000}"/>
+    <hyperlink ref="I3" r:id="rId2" display="mailto:denise.muir@aitheras.com" xr:uid="{00000000-0004-0000-0500-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
@@ -23645,11 +23695,11 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:Y43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A30" sqref="A30:XFD30"/>
+      <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -26063,19 +26113,19 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F3" r:id="rId1" display="mailto:andrewm@aitheras.com"/>
-    <hyperlink ref="I3" r:id="rId2" display="mailto:denise.muir@aitheras.com"/>
+    <hyperlink ref="F3" r:id="rId1" display="mailto:andrewm@aitheras.com" xr:uid="{00000000-0004-0000-0600-000000000000}"/>
+    <hyperlink ref="I3" r:id="rId2" display="mailto:denise.muir@aitheras.com" xr:uid="{00000000-0004-0000-0600-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:Y39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A28" sqref="A28:XFD28"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="I52" sqref="I52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -28283,19 +28333,19 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F3" r:id="rId1" display="mailto:andrewm@aitheras.com"/>
-    <hyperlink ref="I3" r:id="rId2" display="mailto:denise.muir@aitheras.com"/>
+    <hyperlink ref="F3" r:id="rId1" display="mailto:andrewm@aitheras.com" xr:uid="{00000000-0004-0000-0700-000000000000}"/>
+    <hyperlink ref="I3" r:id="rId2" display="mailto:denise.muir@aitheras.com" xr:uid="{00000000-0004-0000-0700-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:Y39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A28" sqref="A28:XFD28"/>
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -30503,8 +30553,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F3" r:id="rId1" display="mailto:andrewm@aitheras.com"/>
-    <hyperlink ref="I3" r:id="rId2" display="mailto:denise.muir@aitheras.com"/>
+    <hyperlink ref="F3" r:id="rId1" display="mailto:andrewm@aitheras.com" xr:uid="{00000000-0004-0000-0800-000000000000}"/>
+    <hyperlink ref="I3" r:id="rId2" display="mailto:denise.muir@aitheras.com" xr:uid="{00000000-0004-0000-0800-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updating the pool names in ERM excel file
</commit_message>
<xml_diff>
--- a/app/data/pools/erm.xlsx
+++ b/app/data/pools/erm.xlsx
@@ -1,24 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dsomalaraju\workspace\discovery\app\data\pools\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0615A28-4B47-47B1-BD01-40872FE4DFFD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="7410" tabRatio="734"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="734" firstSheet="8" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ERM Vendors Master File" sheetId="20" r:id="rId1"/>
-    <sheet name="E1-Desktop Applications" sheetId="1" r:id="rId2"/>
-    <sheet name="E2-Electronic Messages" sheetId="10" r:id="rId3"/>
-    <sheet name="E3-Social Media" sheetId="11" r:id="rId4"/>
-    <sheet name="E4-Cloud Services" sheetId="12" r:id="rId5"/>
-    <sheet name="E5-Websites" sheetId="13" r:id="rId6"/>
-    <sheet name="E6-Digital Media (Photo)" sheetId="14" r:id="rId7"/>
-    <sheet name="E7-Digital Media (Audio)" sheetId="15" r:id="rId8"/>
-    <sheet name="E8-Digital Media (Video)" sheetId="16" r:id="rId9"/>
-    <sheet name="E9-Databases" sheetId="17" r:id="rId10"/>
-    <sheet name="E10-Shared Drives" sheetId="18" r:id="rId11"/>
-    <sheet name="E11-Engineering Drawings" sheetId="19" r:id="rId12"/>
+    <sheet name="E(1)-Desktop Applications" sheetId="1" r:id="rId2"/>
+    <sheet name="E(2)-Electronic Messages" sheetId="10" r:id="rId3"/>
+    <sheet name="E(3)-Social Media" sheetId="11" r:id="rId4"/>
+    <sheet name="E(4)-Cloud Services" sheetId="12" r:id="rId5"/>
+    <sheet name="E(5)-Websites" sheetId="13" r:id="rId6"/>
+    <sheet name="E(6)-Digital Media (Photo)" sheetId="14" r:id="rId7"/>
+    <sheet name="E(7)-Digital Media (Audio)" sheetId="15" r:id="rId8"/>
+    <sheet name="E(8)-Digital Media (Video)" sheetId="16" r:id="rId9"/>
+    <sheet name="E(9)-Databases" sheetId="17" r:id="rId10"/>
+    <sheet name="E(10)-Shared Drives" sheetId="18" r:id="rId11"/>
+    <sheet name="E(11)-Engineering Drawings" sheetId="19" r:id="rId12"/>
     <sheet name="ESRI_MAPINFO_SHEET" sheetId="21" state="veryHidden" r:id="rId13"/>
   </sheets>
   <definedNames>
@@ -1003,7 +1009,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1367,11 +1373,11 @@
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text 2" xfId="4"/>
+    <cellStyle name="Explanatory Text 2" xfId="4" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="3"/>
-    <cellStyle name="Normal 3" xfId="2"/>
+    <cellStyle name="Normal 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="Normal 3" xfId="2" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1447,6 +1453,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -1468,7 +1477,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="EsriDoNotEdit"/>
+        <xdr:cNvPr id="2" name="EsriDoNotEdit">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0C00-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -1588,7 +1603,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1621,9 +1636,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1656,6 +1688,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1831,10 +1880,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AK57"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -6932,10 +6981,10 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AK57"/>
+  <autoFilter ref="A1:AK57" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <hyperlinks>
-    <hyperlink ref="F3" r:id="rId1" display="mailto:andrewm@aitheras.com"/>
-    <hyperlink ref="I3" r:id="rId2" display="mailto:denise.muir@aitheras.com"/>
+    <hyperlink ref="F3" r:id="rId1" display="mailto:andrewm@aitheras.com" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="I3" r:id="rId2" display="mailto:denise.muir@aitheras.com" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
@@ -6943,7 +6992,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:Y52"/>
   <sheetViews>
     <sheetView topLeftCell="A31" workbookViewId="0">
@@ -9903,15 +9952,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F3" r:id="rId1" display="mailto:andrewm@aitheras.com"/>
-    <hyperlink ref="I3" r:id="rId2" display="mailto:denise.muir@aitheras.com"/>
+    <hyperlink ref="F3" r:id="rId1" display="mailto:andrewm@aitheras.com" xr:uid="{00000000-0004-0000-0900-000000000000}"/>
+    <hyperlink ref="I3" r:id="rId2" display="mailto:denise.muir@aitheras.com" xr:uid="{00000000-0004-0000-0900-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:Y46"/>
   <sheetViews>
     <sheetView topLeftCell="A23" workbookViewId="0">
@@ -12511,18 +12560,18 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F3" r:id="rId1" display="mailto:andrewm@aitheras.com"/>
-    <hyperlink ref="I3" r:id="rId2" display="mailto:denise.muir@aitheras.com"/>
+    <hyperlink ref="F3" r:id="rId1" display="mailto:andrewm@aitheras.com" xr:uid="{00000000-0004-0000-0A00-000000000000}"/>
+    <hyperlink ref="I3" r:id="rId2" display="mailto:denise.muir@aitheras.com" xr:uid="{00000000-0004-0000-0A00-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:Y46"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
       <selection activeCell="G54" sqref="G54"/>
     </sheetView>
   </sheetViews>
@@ -15123,15 +15172,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F3" r:id="rId1" display="mailto:andrewm@aitheras.com"/>
-    <hyperlink ref="I3" r:id="rId2" display="mailto:denise.muir@aitheras.com"/>
+    <hyperlink ref="F3" r:id="rId1" display="mailto:andrewm@aitheras.com" xr:uid="{00000000-0004-0000-0B00-000000000000}"/>
+    <hyperlink ref="I3" r:id="rId2" display="mailto:denise.muir@aitheras.com" xr:uid="{00000000-0004-0000-0B00-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -15144,11 +15193,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AB49"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A49" sqref="A49:Y49"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C49" sqref="C49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -17960,8 +18009,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F3" r:id="rId1" display="mailto:andrewm@aitheras.com"/>
-    <hyperlink ref="I3" r:id="rId2" display="mailto:denise.muir@aitheras.com"/>
+    <hyperlink ref="F3" r:id="rId1" display="mailto:andrewm@aitheras.com" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="I3" r:id="rId2" display="mailto:denise.muir@aitheras.com" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
@@ -17969,10 +18018,10 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AB50"/>
   <sheetViews>
-    <sheetView topLeftCell="B37" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
@@ -20824,8 +20873,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F3" r:id="rId1" display="mailto:andrewm@aitheras.com"/>
-    <hyperlink ref="I3" r:id="rId2" display="mailto:denise.muir@aitheras.com"/>
+    <hyperlink ref="F3" r:id="rId1" display="mailto:andrewm@aitheras.com" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="I3" r:id="rId2" display="mailto:denise.muir@aitheras.com" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
@@ -20833,7 +20882,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AB44"/>
   <sheetViews>
     <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
@@ -23361,7 +23410,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AB49"/>
   <sheetViews>
     <sheetView topLeftCell="A24" zoomScaleNormal="100" workbookViewId="0">
@@ -26177,8 +26226,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F3" r:id="rId1" display="mailto:andrewm@aitheras.com"/>
-    <hyperlink ref="I3" r:id="rId2" display="mailto:denise.muir@aitheras.com"/>
+    <hyperlink ref="F3" r:id="rId1" display="mailto:andrewm@aitheras.com" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
+    <hyperlink ref="I3" r:id="rId2" display="mailto:denise.muir@aitheras.com" xr:uid="{00000000-0004-0000-0400-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
@@ -26186,7 +26235,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:AB44"/>
   <sheetViews>
     <sheetView topLeftCell="A20" zoomScaleNormal="100" workbookViewId="0">
@@ -28717,8 +28766,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F3" r:id="rId1" display="mailto:andrewm@aitheras.com"/>
-    <hyperlink ref="I3" r:id="rId2" display="mailto:denise.muir@aitheras.com"/>
+    <hyperlink ref="F3" r:id="rId1" display="mailto:andrewm@aitheras.com" xr:uid="{00000000-0004-0000-0500-000000000000}"/>
+    <hyperlink ref="I3" r:id="rId2" display="mailto:denise.muir@aitheras.com" xr:uid="{00000000-0004-0000-0500-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
@@ -28726,7 +28775,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:Y53"/>
   <sheetViews>
     <sheetView topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
@@ -31730,15 +31779,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F3" r:id="rId1" display="mailto:andrewm@aitheras.com"/>
-    <hyperlink ref="I3" r:id="rId2" display="mailto:denise.muir@aitheras.com"/>
+    <hyperlink ref="F3" r:id="rId1" display="mailto:andrewm@aitheras.com" xr:uid="{00000000-0004-0000-0600-000000000000}"/>
+    <hyperlink ref="I3" r:id="rId2" display="mailto:denise.muir@aitheras.com" xr:uid="{00000000-0004-0000-0600-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:Y49"/>
   <sheetViews>
     <sheetView topLeftCell="A24" workbookViewId="0">
@@ -34511,15 +34560,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F3" r:id="rId1" display="mailto:andrewm@aitheras.com"/>
-    <hyperlink ref="I3" r:id="rId2" display="mailto:denise.muir@aitheras.com"/>
+    <hyperlink ref="F3" r:id="rId1" display="mailto:andrewm@aitheras.com" xr:uid="{00000000-0004-0000-0700-000000000000}"/>
+    <hyperlink ref="I3" r:id="rId2" display="mailto:denise.muir@aitheras.com" xr:uid="{00000000-0004-0000-0700-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:Y49"/>
   <sheetViews>
     <sheetView topLeftCell="A28" workbookViewId="0">
@@ -37290,8 +37339,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F3" r:id="rId1" display="mailto:andrewm@aitheras.com"/>
-    <hyperlink ref="I3" r:id="rId2" display="mailto:denise.muir@aitheras.com"/>
+    <hyperlink ref="F3" r:id="rId1" display="mailto:andrewm@aitheras.com" xr:uid="{00000000-0004-0000-0800-000000000000}"/>
+    <hyperlink ref="I3" r:id="rId2" display="mailto:denise.muir@aitheras.com" xr:uid="{00000000-0004-0000-0800-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated pool records (converted duns number field error) on ERM vehicle data
</commit_message>
<xml_diff>
--- a/app/data/pools/erm.xlsx
+++ b/app/data/pools/erm.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dsomalaraju\workspace\discovery\app\data\pools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0615A28-4B47-47B1-BD01-40872FE4DFFD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5053BBC9-0F9E-4A44-BDB9-12E70602808A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="734" firstSheet="8" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="734" firstSheet="6" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ERM Vendors Master File" sheetId="20" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8133" uniqueCount="323">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8093" uniqueCount="324">
   <si>
     <t>ContractorName</t>
   </si>
@@ -1005,6 +1005,9 @@
   <si>
     <t>joseph.dooley@nccsite.com</t>
   </si>
+  <si>
+    <t>133097183</t>
+  </si>
 </sst>
 </file>
 
@@ -6995,8 +6998,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:Y52"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="A52" sqref="A52:Y52"/>
+    <sheetView topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7593,8 +7596,8 @@
       <c r="B11" s="19" t="s">
         <v>128</v>
       </c>
-      <c r="C11" s="21" t="s">
-        <v>234</v>
+      <c r="C11" s="22">
+        <v>78409916</v>
       </c>
       <c r="D11" s="17"/>
       <c r="E11" s="19" t="s">
@@ -7711,8 +7714,8 @@
       <c r="B13" s="19" t="s">
         <v>246</v>
       </c>
-      <c r="C13" s="21" t="s">
-        <v>247</v>
+      <c r="C13" s="22">
+        <v>786283130</v>
       </c>
       <c r="D13" s="19" t="s">
         <v>248</v>
@@ -8102,8 +8105,8 @@
       <c r="B20" s="19" t="s">
         <v>236</v>
       </c>
-      <c r="C20" s="21" t="s">
-        <v>237</v>
+      <c r="C20" s="22">
+        <v>12290920</v>
       </c>
       <c r="D20" s="19"/>
       <c r="E20" s="19" t="s">
@@ -8214,8 +8217,8 @@
       <c r="B22" s="19" t="s">
         <v>157</v>
       </c>
-      <c r="C22" s="21" t="s">
-        <v>184</v>
+      <c r="C22" s="22">
+        <v>120439869</v>
       </c>
       <c r="D22" s="19" t="s">
         <v>158</v>
@@ -8501,8 +8504,8 @@
       <c r="B27" s="19" t="s">
         <v>175</v>
       </c>
-      <c r="C27" s="21" t="s">
-        <v>176</v>
+      <c r="C27" s="22">
+        <v>1742662</v>
       </c>
       <c r="D27" s="19" t="s">
         <v>177</v>
@@ -9352,8 +9355,8 @@
       <c r="B42" s="19" t="s">
         <v>208</v>
       </c>
-      <c r="C42" s="21" t="s">
-        <v>254</v>
+      <c r="C42" s="22">
+        <v>79120324</v>
       </c>
       <c r="D42" s="19" t="s">
         <v>255</v>
@@ -9521,8 +9524,8 @@
       <c r="B45" s="19" t="s">
         <v>276</v>
       </c>
-      <c r="C45" s="21" t="s">
-        <v>277</v>
+      <c r="C45" s="22">
+        <v>78830982</v>
       </c>
       <c r="D45" s="17" t="s">
         <v>278</v>
@@ -9576,8 +9579,8 @@
       <c r="B46" s="21" t="s">
         <v>281</v>
       </c>
-      <c r="C46" s="21" t="s">
-        <v>292</v>
+      <c r="C46" s="22">
+        <v>86512134</v>
       </c>
       <c r="D46" s="17" t="s">
         <v>282</v>
@@ -9759,8 +9762,8 @@
       <c r="B49" s="44" t="s">
         <v>295</v>
       </c>
-      <c r="C49" s="45" t="s">
-        <v>296</v>
+      <c r="C49" s="48">
+        <v>66493946</v>
       </c>
       <c r="D49" s="43" t="s">
         <v>297</v>
@@ -9812,8 +9815,8 @@
       <c r="B50" s="44" t="s">
         <v>305</v>
       </c>
-      <c r="C50" s="45" t="s">
-        <v>308</v>
+      <c r="C50" s="48">
+        <v>362904331</v>
       </c>
       <c r="D50" s="43"/>
       <c r="E50" s="44" t="s">
@@ -9963,8 +9966,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:Y46"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="A46" sqref="A46:Y46"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -10339,8 +10342,8 @@
       <c r="B7" s="19" t="s">
         <v>263</v>
       </c>
-      <c r="C7" s="21" t="s">
-        <v>241</v>
+      <c r="C7" s="22">
+        <v>101471444</v>
       </c>
       <c r="D7" s="17" t="s">
         <v>242</v>
@@ -10667,8 +10670,8 @@
       <c r="B13" s="19" t="s">
         <v>128</v>
       </c>
-      <c r="C13" s="21" t="s">
-        <v>234</v>
+      <c r="C13" s="22">
+        <v>78409916</v>
       </c>
       <c r="D13" s="17"/>
       <c r="E13" s="19" t="s">
@@ -10785,8 +10788,8 @@
       <c r="B15" s="19" t="s">
         <v>246</v>
       </c>
-      <c r="C15" s="21" t="s">
-        <v>247</v>
+      <c r="C15" s="22">
+        <v>786283130</v>
       </c>
       <c r="D15" s="19" t="s">
         <v>248</v>
@@ -11064,8 +11067,8 @@
       <c r="B20" s="19" t="s">
         <v>236</v>
       </c>
-      <c r="C20" s="21" t="s">
-        <v>237</v>
+      <c r="C20" s="22">
+        <v>12290920</v>
       </c>
       <c r="D20" s="19"/>
       <c r="E20" s="19" t="s">
@@ -11117,8 +11120,8 @@
       <c r="B21" s="19" t="s">
         <v>157</v>
       </c>
-      <c r="C21" s="21" t="s">
-        <v>184</v>
+      <c r="C21" s="22">
+        <v>120439869</v>
       </c>
       <c r="D21" s="19" t="s">
         <v>158</v>
@@ -11343,8 +11346,8 @@
       <c r="B25" s="19" t="s">
         <v>175</v>
       </c>
-      <c r="C25" s="21" t="s">
-        <v>176</v>
+      <c r="C25" s="22">
+        <v>1742662</v>
       </c>
       <c r="D25" s="19" t="s">
         <v>177</v>
@@ -12074,8 +12077,8 @@
       <c r="B38" s="19" t="s">
         <v>208</v>
       </c>
-      <c r="C38" s="21" t="s">
-        <v>254</v>
+      <c r="C38" s="22">
+        <v>79120324</v>
       </c>
       <c r="D38" s="19" t="s">
         <v>255</v>
@@ -12367,8 +12370,8 @@
       <c r="B43" s="44" t="s">
         <v>295</v>
       </c>
-      <c r="C43" s="45" t="s">
-        <v>296</v>
+      <c r="C43" s="48">
+        <v>66493946</v>
       </c>
       <c r="D43" s="43" t="s">
         <v>297</v>
@@ -12420,8 +12423,8 @@
       <c r="B44" s="44" t="s">
         <v>305</v>
       </c>
-      <c r="C44" s="45" t="s">
-        <v>308</v>
+      <c r="C44" s="48">
+        <v>362904331</v>
       </c>
       <c r="D44" s="43"/>
       <c r="E44" s="44" t="s">
@@ -12571,7 +12574,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:Y46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+    <sheetView topLeftCell="A38" workbookViewId="0">
       <selection activeCell="G54" sqref="G54"/>
     </sheetView>
   </sheetViews>
@@ -15196,7 +15199,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AB49"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A30" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C49" sqref="C49"/>
     </sheetView>
   </sheetViews>
@@ -18021,8 +18024,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AB50"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B50" sqref="B50"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -18139,7 +18142,7 @@
       <c r="B2" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="C2" s="21">
+      <c r="C2" s="22">
         <v>143975295</v>
       </c>
       <c r="D2" s="20"/>
@@ -18255,7 +18258,7 @@
       <c r="B4" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="C4" s="21">
+      <c r="C4" s="22">
         <v>126624399</v>
       </c>
       <c r="D4" s="20"/>
@@ -18306,7 +18309,7 @@
       <c r="B5" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="C5" s="21">
+      <c r="C5" s="22">
         <v>122477008</v>
       </c>
       <c r="D5" s="20" t="s">
@@ -18363,7 +18366,7 @@
       <c r="B6" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="C6" s="21">
+      <c r="C6" s="22">
         <v>133097183</v>
       </c>
       <c r="D6" s="20"/>
@@ -18422,8 +18425,8 @@
       <c r="B7" s="19" t="s">
         <v>263</v>
       </c>
-      <c r="C7" s="21" t="s">
-        <v>241</v>
+      <c r="C7" s="22">
+        <v>101471444</v>
       </c>
       <c r="D7" s="17" t="s">
         <v>242</v>
@@ -18750,8 +18753,8 @@
       <c r="B13" s="19" t="s">
         <v>128</v>
       </c>
-      <c r="C13" s="21" t="s">
-        <v>234</v>
+      <c r="C13" s="22">
+        <v>78409916</v>
       </c>
       <c r="D13" s="17"/>
       <c r="E13" s="19" t="s">
@@ -18868,8 +18871,8 @@
       <c r="B15" s="19" t="s">
         <v>246</v>
       </c>
-      <c r="C15" s="21" t="s">
-        <v>247</v>
+      <c r="C15" s="22">
+        <v>786283130</v>
       </c>
       <c r="D15" s="19" t="s">
         <v>248</v>
@@ -19259,8 +19262,8 @@
       <c r="B22" s="19" t="s">
         <v>236</v>
       </c>
-      <c r="C22" s="21" t="s">
-        <v>237</v>
+      <c r="C22" s="22">
+        <v>12290920</v>
       </c>
       <c r="D22" s="19"/>
       <c r="E22" s="19" t="s">
@@ -19371,8 +19374,8 @@
       <c r="B24" s="19" t="s">
         <v>157</v>
       </c>
-      <c r="C24" s="21" t="s">
-        <v>184</v>
+      <c r="C24" s="22">
+        <v>120439869</v>
       </c>
       <c r="D24" s="19" t="s">
         <v>158</v>
@@ -19542,8 +19545,8 @@
       <c r="B27" s="19" t="s">
         <v>175</v>
       </c>
-      <c r="C27" s="21" t="s">
-        <v>176</v>
+      <c r="C27" s="22">
+        <v>1742662</v>
       </c>
       <c r="D27" s="19" t="s">
         <v>177</v>
@@ -19865,7 +19868,7 @@
         <v>45116</v>
       </c>
     </row>
-    <row r="33" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A33" s="17" t="s">
         <v>106</v>
       </c>
@@ -19926,7 +19929,7 @@
         <v>44660</v>
       </c>
     </row>
-    <row r="34" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A34" s="17" t="s">
         <v>108</v>
       </c>
@@ -19979,7 +19982,7 @@
         <v>44842</v>
       </c>
     </row>
-    <row r="35" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A35" s="23" t="s">
         <v>109</v>
       </c>
@@ -20038,7 +20041,7 @@
         <v>44469</v>
       </c>
     </row>
-    <row r="36" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A36" s="19" t="s">
         <v>111</v>
       </c>
@@ -20093,7 +20096,7 @@
         <v>45158</v>
       </c>
     </row>
-    <row r="37" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A37" s="17" t="s">
         <v>113</v>
       </c>
@@ -20150,7 +20153,7 @@
         <v>43591</v>
       </c>
     </row>
-    <row r="38" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A38" s="17" t="s">
         <v>114</v>
       </c>
@@ -20213,7 +20216,7 @@
         <v>43935</v>
       </c>
     </row>
-    <row r="39" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A39" s="17" t="s">
         <v>116</v>
       </c>
@@ -20266,15 +20269,15 @@
         <v>43666</v>
       </c>
     </row>
-    <row r="40" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A40" s="17" t="s">
         <v>252</v>
       </c>
       <c r="B40" s="19" t="s">
         <v>208</v>
       </c>
-      <c r="C40" s="21" t="s">
-        <v>254</v>
+      <c r="C40" s="22">
+        <v>79120324</v>
       </c>
       <c r="D40" s="19" t="s">
         <v>255</v>
@@ -20327,7 +20330,7 @@
         <v>44269</v>
       </c>
     </row>
-    <row r="41" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A41" s="17" t="s">
         <v>251</v>
       </c>
@@ -20380,7 +20383,7 @@
         <v>44277</v>
       </c>
     </row>
-    <row r="42" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A42" s="17" t="s">
         <v>253</v>
       </c>
@@ -20435,15 +20438,15 @@
         <v>45351</v>
       </c>
     </row>
-    <row r="43" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A43" s="17" t="s">
         <v>265</v>
       </c>
       <c r="B43" s="19" t="s">
         <v>276</v>
       </c>
-      <c r="C43" s="21" t="s">
-        <v>277</v>
+      <c r="C43" s="22">
+        <v>78830982</v>
       </c>
       <c r="D43" s="17" t="s">
         <v>278</v>
@@ -20490,15 +20493,15 @@
         <v>45516</v>
       </c>
     </row>
-    <row r="44" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A44" s="17" t="s">
         <v>266</v>
       </c>
       <c r="B44" s="21" t="s">
         <v>281</v>
       </c>
-      <c r="C44" s="21" t="s">
-        <v>292</v>
+      <c r="C44" s="22">
+        <v>86512134</v>
       </c>
       <c r="D44" s="17" t="s">
         <v>282</v>
@@ -20549,7 +20552,7 @@
         <v>45482</v>
       </c>
     </row>
-    <row r="45" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A45" s="19" t="s">
         <v>267</v>
       </c>
@@ -20612,7 +20615,7 @@
         <v>45453</v>
       </c>
     </row>
-    <row r="46" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A46" s="17" t="s">
         <v>268</v>
       </c>
@@ -20673,15 +20676,15 @@
         <v>43725</v>
       </c>
     </row>
-    <row r="47" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A47" s="43" t="s">
         <v>293</v>
       </c>
       <c r="B47" s="44" t="s">
         <v>295</v>
       </c>
-      <c r="C47" s="45" t="s">
-        <v>296</v>
+      <c r="C47" s="48">
+        <v>66493946</v>
       </c>
       <c r="D47" s="43" t="s">
         <v>297</v>
@@ -20726,35 +20729,38 @@
         <v>45397</v>
       </c>
     </row>
-    <row r="48" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="B48" s="43" t="s">
+    <row r="48" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A48" s="43" t="s">
         <v>304</v>
       </c>
-      <c r="C48" s="44" t="s">
+      <c r="B48" s="44" t="s">
         <v>305</v>
       </c>
-      <c r="D48" s="45" t="s">
-        <v>308</v>
-      </c>
-      <c r="E48" s="43"/>
+      <c r="C48" s="48">
+        <v>362904331</v>
+      </c>
+      <c r="D48" s="43"/>
+      <c r="E48" s="44" t="s">
+        <v>310</v>
+      </c>
       <c r="F48" s="44" t="s">
-        <v>310</v>
-      </c>
-      <c r="G48" s="44" t="s">
         <v>309</v>
       </c>
+      <c r="G48" s="46"/>
       <c r="H48" s="46"/>
       <c r="I48" s="46"/>
       <c r="J48" s="46"/>
       <c r="K48" s="46"/>
-      <c r="L48" s="46"/>
-      <c r="M48" s="47"/>
+      <c r="L48" s="47"/>
+      <c r="M48" s="46"/>
       <c r="N48" s="46"/>
       <c r="O48" s="46"/>
       <c r="P48" s="46"/>
       <c r="Q48" s="46"/>
       <c r="R48" s="46"/>
-      <c r="S48" s="46"/>
+      <c r="S48" s="46" t="s">
+        <v>275</v>
+      </c>
       <c r="T48" s="46" t="s">
         <v>275</v>
       </c>
@@ -20770,40 +20776,38 @@
       <c r="X48" s="46" t="s">
         <v>275</v>
       </c>
-      <c r="Y48" s="46" t="s">
-        <v>275</v>
-      </c>
-      <c r="Z48" s="47">
+      <c r="Y48" s="47">
         <v>45663</v>
       </c>
     </row>
-    <row r="49" spans="2:26" x14ac:dyDescent="0.2">
-      <c r="B49" s="43" t="s">
+    <row r="49" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A49" s="43" t="s">
         <v>306</v>
       </c>
-      <c r="C49" s="44" t="s">
+      <c r="B49" s="44" t="s">
         <v>148</v>
       </c>
-      <c r="D49" s="44">
+      <c r="C49" s="44">
         <v>117201286</v>
       </c>
-      <c r="E49" s="44"/>
-      <c r="F49" s="44" t="s">
+      <c r="D49" s="44"/>
+      <c r="E49" s="44" t="s">
         <v>318</v>
       </c>
-      <c r="G49" s="44"/>
+      <c r="F49" s="44"/>
+      <c r="G49" s="46"/>
       <c r="H49" s="46"/>
       <c r="I49" s="46"/>
-      <c r="J49" s="46"/>
-      <c r="K49" s="46" t="s">
-        <v>20</v>
-      </c>
-      <c r="L49" s="46"/>
-      <c r="M49" s="47"/>
-      <c r="N49" s="46"/>
-      <c r="O49" s="46" t="s">
-        <v>20</v>
-      </c>
+      <c r="J49" s="46" t="s">
+        <v>20</v>
+      </c>
+      <c r="K49" s="46"/>
+      <c r="L49" s="47"/>
+      <c r="M49" s="46"/>
+      <c r="N49" s="46" t="s">
+        <v>20</v>
+      </c>
+      <c r="O49" s="46"/>
       <c r="P49" s="46"/>
       <c r="Q49" s="46"/>
       <c r="R49" s="46"/>
@@ -20813,30 +20817,30 @@
       <c r="V49" s="46"/>
       <c r="W49" s="46"/>
       <c r="X49" s="46"/>
-      <c r="Y49" s="46"/>
-      <c r="Z49" s="47">
+      <c r="Y49" s="47">
         <v>45695</v>
       </c>
     </row>
-    <row r="50" spans="2:26" x14ac:dyDescent="0.2">
-      <c r="B50" s="43" t="s">
+    <row r="50" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A50" s="43" t="s">
         <v>307</v>
       </c>
-      <c r="C50" s="44" t="s">
+      <c r="B50" s="44" t="s">
         <v>319</v>
       </c>
-      <c r="D50" s="48">
+      <c r="C50" s="48">
         <v>125132048</v>
       </c>
+      <c r="D50" s="44" t="s">
+        <v>320</v>
+      </c>
       <c r="E50" s="44" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="F50" s="44" t="s">
-        <v>321</v>
-      </c>
-      <c r="G50" s="44" t="s">
         <v>322</v>
       </c>
+      <c r="G50" s="46"/>
       <c r="H50" s="46"/>
       <c r="I50" s="46"/>
       <c r="J50" s="46"/>
@@ -20848,7 +20852,9 @@
       <c r="P50" s="46"/>
       <c r="Q50" s="46"/>
       <c r="R50" s="46"/>
-      <c r="S50" s="46"/>
+      <c r="S50" s="46" t="s">
+        <v>20</v>
+      </c>
       <c r="T50" s="46" t="s">
         <v>20</v>
       </c>
@@ -20864,10 +20870,7 @@
       <c r="X50" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="Y50" s="46" t="s">
-        <v>20</v>
-      </c>
-      <c r="Z50" s="47">
+      <c r="Y50" s="47">
         <v>45656</v>
       </c>
     </row>
@@ -20885,7 +20888,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AB44"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A29" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A44" sqref="A44:Y44"/>
     </sheetView>
   </sheetViews>
@@ -23413,7 +23416,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AB49"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A33" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D56" sqref="D56"/>
     </sheetView>
   </sheetViews>
@@ -26238,8 +26241,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:AB44"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A44" sqref="A44:Y44"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -26580,8 +26583,8 @@
       <c r="B6" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="C6" s="21">
-        <v>133097183</v>
+      <c r="C6" s="21" t="s">
+        <v>323</v>
       </c>
       <c r="D6" s="17"/>
       <c r="E6" s="17" t="s">
@@ -31791,7 +31794,7 @@
   <dimension ref="A1:Y49"/>
   <sheetViews>
     <sheetView topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="A49" sqref="A49:Y49"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -34571,13 +34574,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:Y49"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="A49" sqref="A49:Y49"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="I43" sqref="I43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="11.109375" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
@@ -34947,8 +34953,8 @@
       <c r="B7" s="19" t="s">
         <v>263</v>
       </c>
-      <c r="C7" s="21" t="s">
-        <v>241</v>
+      <c r="C7" s="22">
+        <v>101471444</v>
       </c>
       <c r="D7" s="17" t="s">
         <v>242</v>
@@ -35275,8 +35281,8 @@
       <c r="B13" s="19" t="s">
         <v>128</v>
       </c>
-      <c r="C13" s="21" t="s">
-        <v>234</v>
+      <c r="C13" s="22">
+        <v>78409916</v>
       </c>
       <c r="D13" s="17"/>
       <c r="E13" s="19" t="s">
@@ -35393,8 +35399,8 @@
       <c r="B15" s="19" t="s">
         <v>246</v>
       </c>
-      <c r="C15" s="21" t="s">
-        <v>247</v>
+      <c r="C15" s="22">
+        <v>786283130</v>
       </c>
       <c r="D15" s="19" t="s">
         <v>248</v>
@@ -35672,8 +35678,8 @@
       <c r="B20" s="19" t="s">
         <v>236</v>
       </c>
-      <c r="C20" s="21" t="s">
-        <v>237</v>
+      <c r="C20" s="22">
+        <v>12290920</v>
       </c>
       <c r="D20" s="19"/>
       <c r="E20" s="19" t="s">
@@ -35725,8 +35731,8 @@
       <c r="B21" s="19" t="s">
         <v>157</v>
       </c>
-      <c r="C21" s="21" t="s">
-        <v>184</v>
+      <c r="C21" s="22">
+        <v>120439869</v>
       </c>
       <c r="D21" s="19" t="s">
         <v>158</v>
@@ -35951,8 +35957,8 @@
       <c r="B25" s="19" t="s">
         <v>175</v>
       </c>
-      <c r="C25" s="21" t="s">
-        <v>176</v>
+      <c r="C25" s="22">
+        <v>1742662</v>
       </c>
       <c r="D25" s="19" t="s">
         <v>177</v>
@@ -36741,8 +36747,8 @@
       <c r="B39" s="19" t="s">
         <v>208</v>
       </c>
-      <c r="C39" s="21" t="s">
-        <v>254</v>
+      <c r="C39" s="22">
+        <v>79120324</v>
       </c>
       <c r="D39" s="19" t="s">
         <v>255</v>
@@ -36910,8 +36916,8 @@
       <c r="B42" s="19" t="s">
         <v>276</v>
       </c>
-      <c r="C42" s="21" t="s">
-        <v>277</v>
+      <c r="C42" s="22">
+        <v>78830982</v>
       </c>
       <c r="D42" s="17" t="s">
         <v>278</v>
@@ -36962,12 +36968,11 @@
       <c r="A43" s="17" t="s">
         <v>266</v>
       </c>
-      <c r="B43" s="19"/>
-      <c r="C43" s="21" t="s">
+      <c r="B43" s="22" t="s">
         <v>281</v>
       </c>
-      <c r="D43" s="21" t="s">
-        <v>292</v>
+      <c r="C43" s="22">
+        <v>86512134</v>
       </c>
       <c r="E43" s="19" t="s">
         <v>283</v>
@@ -36981,7 +36986,7 @@
       <c r="H43" s="7" t="s">
         <v>283</v>
       </c>
-      <c r="I43" s="7" t="s">
+      <c r="I43" s="19" t="s">
         <v>286</v>
       </c>
       <c r="J43" s="7"/>
@@ -37146,8 +37151,8 @@
       <c r="B46" s="44" t="s">
         <v>295</v>
       </c>
-      <c r="C46" s="45" t="s">
-        <v>296</v>
+      <c r="C46" s="48">
+        <v>66493946</v>
       </c>
       <c r="D46" s="43" t="s">
         <v>297</v>
@@ -37199,8 +37204,8 @@
       <c r="B47" s="44" t="s">
         <v>305</v>
       </c>
-      <c r="C47" s="45" t="s">
-        <v>308</v>
+      <c r="C47" s="48">
+        <v>362904331</v>
       </c>
       <c r="D47" s="43"/>
       <c r="E47" s="44" t="s">
@@ -37341,7 +37346,9 @@
   <hyperlinks>
     <hyperlink ref="F3" r:id="rId1" display="mailto:andrewm@aitheras.com" xr:uid="{00000000-0004-0000-0800-000000000000}"/>
     <hyperlink ref="I3" r:id="rId2" display="mailto:denise.muir@aitheras.com" xr:uid="{00000000-0004-0000-0800-000001000000}"/>
+    <hyperlink ref="I43" r:id="rId3" xr:uid="{AAFD3D28-1BC5-4399-A02A-44CDDE5521DD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updating ERM vendors in PROD
</commit_message>
<xml_diff>
--- a/app/data/pools/erm.xlsx
+++ b/app/data/pools/erm.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\discovery\app\data\pools\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dsomalaraju\Desktop\Discovery\OLD data\New\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B96A64D6-C006-47C0-A077-0A21CAAB954D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05160E38-0B39-4C2F-9BD3-5654A87E8440}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" tabRatio="674" firstSheet="7" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="674" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ERM Vendors Master File" sheetId="20" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7636" uniqueCount="294">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7635" uniqueCount="294">
   <si>
     <t>ContractorName</t>
   </si>
@@ -6497,7 +6497,7 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:AK52" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
-  <sortState ref="A2:AK52">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AK52">
     <sortCondition ref="A2:A52"/>
   </sortState>
   <hyperlinks>
@@ -9271,7 +9271,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:Y48">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Y48">
     <sortCondition ref="A2:A48"/>
   </sortState>
   <hyperlinks>
@@ -11687,7 +11687,7 @@
       <c r="C43" s="53"/>
     </row>
   </sheetData>
-  <sortState ref="A2:Y42">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Y42">
     <sortCondition ref="A2:A42"/>
   </sortState>
   <hyperlinks>
@@ -11702,7 +11702,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:Y44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" activeCellId="1" sqref="C3:C44 C2"/>
     </sheetView>
   </sheetViews>
@@ -14208,7 +14208,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:Y44">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Y44">
     <sortCondition ref="A2:A44"/>
   </sortState>
   <hyperlinks>
@@ -14236,7 +14236,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AB46"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
@@ -16903,7 +16903,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:Y46">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Y46">
     <sortCondition ref="A2:A46"/>
   </sortState>
   <hyperlinks>
@@ -16919,8 +16919,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AB46"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -17709,8 +17709,8 @@
       <c r="B14" s="19" t="s">
         <v>128</v>
       </c>
-      <c r="C14" s="22" t="s">
-        <v>234</v>
+      <c r="C14" s="22">
+        <v>78409916</v>
       </c>
       <c r="D14" s="17"/>
       <c r="E14" s="19" t="s">
@@ -19572,7 +19572,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:Y46">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Y46">
     <sortCondition ref="A2:A46"/>
   </sortState>
   <hyperlinks>
@@ -21909,7 +21909,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:Y40">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Y40">
     <sortCondition ref="A2:A40"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -24535,7 +24535,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:Y45">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Y45">
     <sortCondition ref="A2:A45"/>
   </sortState>
   <hyperlinks>
@@ -26936,7 +26936,7 @@
       <c r="C42" s="54"/>
     </row>
   </sheetData>
-  <sortState ref="A2:Y41">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Y41">
     <sortCondition ref="A2:A41"/>
   </sortState>
   <hyperlinks>
@@ -29757,7 +29757,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:Y49">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Y49">
     <sortCondition ref="A2:A49"/>
   </sortState>
   <hyperlinks>
@@ -32343,7 +32343,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:Y45">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Y45">
     <sortCondition ref="A2:A45"/>
   </sortState>
   <hyperlinks>
@@ -34929,7 +34929,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:Y45">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Y45">
     <sortCondition ref="A2:A45"/>
   </sortState>
   <hyperlinks>

</xml_diff>